<commit_message>
Added multiple files and updated codes
</commit_message>
<xml_diff>
--- a/src/test/resources/Test_Cases_and_Scenarios.xlsx
+++ b/src/test/resources/Test_Cases_and_Scenarios.xlsx
@@ -3,20 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1f443580377edc98/Documents/gitDevelopmentTesting/API-UI-Test_Automation/src/test/resources/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="144" documentId="11_F25DC773A252ABDACC1048A2615D55C65ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19E4DF11-548B-408E-894C-B1D5191BBDFE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{67EF5009-DE27-45ED-B930-62214168B263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UI Test cases" sheetId="1" r:id="rId1"/>
     <sheet name="API Test cases" sheetId="2" r:id="rId2"/>
+    <sheet name="Test Data" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
   <si>
     <t>Step 1:-</t>
   </si>
@@ -134,6 +131,27 @@
   </si>
   <si>
     <t>TC - 05 - Verify menu bar and its functionality</t>
+  </si>
+  <si>
+    <t>Dropdown Data</t>
+  </si>
+  <si>
+    <t>Name (Z to A)</t>
+  </si>
+  <si>
+    <t>Price (high to low)</t>
+  </si>
+  <si>
+    <t>Price (low to high)</t>
+  </si>
+  <si>
+    <t>Checkout Information</t>
+  </si>
+  <si>
+    <t>Dinesh</t>
+  </si>
+  <si>
+    <t>Nimmala</t>
   </si>
 </sst>
 </file>
@@ -247,10 +265,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -518,7 +532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="A1:D23"/>
     </sheetView>
   </sheetViews>
@@ -821,4 +835,55 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C01D040-761B-44FC-92A7-65D5370ED420}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4">
+        <v>505050</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>